<commit_message>
Jeg har tenkt å refaktorere Item til å bli interface Item<T>
</commit_message>
<xml_diff>
--- a/civilization/src/main/resources/assets/gamedata-faf-waw.xlsx
+++ b/civilization/src/main/resources/assets/gamedata-faf-waw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Civ" sheetId="1" r:id="rId1"/>
@@ -1566,7 +1566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1802,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,7 +2262,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2449,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2475,7 +2475,7 @@
       </c>
       <c r="B2" s="2">
         <f ca="1">RAND()</f>
-        <v>0.38612398108597412</v>
+        <v>0.63067811233014115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2484,7 +2484,7 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RAND()</f>
-        <v>0.68365416744083196</v>
+        <v>0.55210034023805887</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
       </c>
       <c r="B4" s="2">
         <f ca="1">RAND()</f>
-        <v>0.40570804085946066</v>
+        <v>5.3011397440666852E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="B5" s="2">
         <f ca="1">RAND()</f>
-        <v>0.16703374626941658</v>
+        <v>0.43511889523821967</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2511,7 +2511,7 @@
       </c>
       <c r="B6" s="2">
         <f ca="1">RAND()</f>
-        <v>0.89637810637027659</v>
+        <v>0.34599895173895823</v>
       </c>
     </row>
   </sheetData>
@@ -3236,7 +3236,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3775,12 +3775,15 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="6.85546875"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
@@ -4555,7 +4558,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>